<commit_message>
Bluetooth and TMP117 integrated
</commit_message>
<xml_diff>
--- a/questions/Assignment6-ClientCommandTableForA7.xlsx
+++ b/questions/Assignment6-ClientCommandTableForA7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjahn\SimplicityStudio\v5_workspace\ecen5823-assignment6-Jahnavi-pinnamaneni\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF30E7CD-DDC4-4CE0-BEF3-099F6D1EBAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A0F444-988D-4ECC-9CAD-EBC868186713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-10780" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Client Command Table for A7</t>
   </si>
@@ -177,9 +177,6 @@
     </r>
   </si>
   <si>
-    <t>sl_bt_gatt_discover_primary_services_by_uuid()</t>
-  </si>
-  <si>
     <t>X Save connection handle</t>
   </si>
   <si>
@@ -192,6 +189,10 @@
     <t>We get this event when it’s ok to call the next GATT command. It’s a good idea to check for returned error codes. This would be a great event to use to sequence your new state machine.
 sl_bt_gatt_discover_characteristics_by_uuid()
 sl_bt_gatt_set_charecteristic_notification()</t>
+  </si>
+  <si>
+    <t>sl_bt_gatt_discover_primary_services_by_uuid()
+sl_bt_scanner_stop()</t>
   </si>
 </sst>
 </file>
@@ -601,22 +602,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>176530</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1296288</xdr:rowOff>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>90254</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1053961</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>846799</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>359271</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>134837</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F67A0F9-FC09-C4D8-A54F-418A2F29AF3B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C40E9E57-457F-779D-1B17-2CBBA9711977}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -632,8 +633,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13702030" y="1632838"/>
-          <a:ext cx="8700631" cy="5062311"/>
+          <a:off x="13616940" y="90254"/>
+          <a:ext cx="18190071" cy="10590663"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1725,8 +1726,8 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1869,17 +1870,17 @@
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="17" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F12" s="16"/>
     </row>
@@ -1900,7 +1901,9 @@
       <c r="D14" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="16"/>
+      <c r="E14" s="16" t="s">
+        <v>16</v>
+      </c>
       <c r="F14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1971,7 +1974,7 @@
         <v>33</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F21" s="20" t="s">
         <v>26</v>
@@ -1992,7 +1995,7 @@
       </c>
       <c r="C23" s="16"/>
       <c r="D23" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>28</v>
@@ -2014,7 +2017,7 @@
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>30</v>

</xml_diff>